<commit_message>
drafted trial selection chapter and added consort diagrams to supplement
</commit_message>
<xml_diff>
--- a/tables/helper_tables.xlsx
+++ b/tables/helper_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janickweberpals/Documents/Projects/encore-process-paper/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E290701-E1D1-644E-A6CC-A03E35313BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E176BD46-8E3E-4C4B-99EB-8B2198800D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,9 +191,6 @@
     <t>NCT01673867</t>
   </si>
   <si>
-    <t>CheckMate057</t>
-  </si>
-  <si>
     <t>CheckMate9LA</t>
   </si>
   <si>
@@ -335,10 +332,13 @@
     <t>Relapsed or refractory</t>
   </si>
   <si>
-    <t>Metastatic non-squamous</t>
-  </si>
-  <si>
     <t>pembrolizumab versus standard of care</t>
+  </si>
+  <si>
+    <t>CheckMate017/057</t>
+  </si>
+  <si>
+    <t>Metastatic squamous/non-squamous</t>
   </si>
 </sst>
 </file>
@@ -1361,14 +1361,14 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="71.1640625" bestFit="1" customWidth="1"/>
@@ -1388,7 +1388,7 @@
         <v>45</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>46</v>
@@ -1405,13 +1405,13 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1422,16 +1422,16 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1442,16 +1442,16 @@
         <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1459,19 +1459,19 @@
         <v>48</v>
       </c>
       <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
         <v>65</v>
       </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1479,19 +1479,19 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
         <v>67</v>
       </c>
-      <c r="C6" t="s">
-        <v>68</v>
-      </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1499,19 +1499,19 @@
         <v>48</v>
       </c>
       <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
         <v>69</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" t="s">
         <v>70</v>
-      </c>
-      <c r="D7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1519,19 +1519,19 @@
         <v>49</v>
       </c>
       <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
         <v>84</v>
       </c>
-      <c r="C8" t="s">
-        <v>85</v>
-      </c>
       <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" t="s">
         <v>91</v>
       </c>
-      <c r="E8" t="s">
-        <v>92</v>
-      </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1539,19 +1539,19 @@
         <v>49</v>
       </c>
       <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" t="s">
         <v>86</v>
       </c>
-      <c r="C9" t="s">
-        <v>87</v>
-      </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1559,19 +1559,19 @@
         <v>49</v>
       </c>
       <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
         <v>88</v>
       </c>
-      <c r="C10" t="s">
-        <v>89</v>
-      </c>
       <c r="D10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" t="s">
         <v>94</v>
       </c>
-      <c r="E10" t="s">
-        <v>95</v>
-      </c>
       <c r="F10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1579,19 +1579,19 @@
         <v>50</v>
       </c>
       <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
         <v>78</v>
       </c>
-      <c r="C11" t="s">
-        <v>79</v>
-      </c>
       <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" t="s">
         <v>97</v>
       </c>
-      <c r="E11" t="s">
-        <v>98</v>
-      </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1599,19 +1599,19 @@
         <v>50</v>
       </c>
       <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
         <v>80</v>
       </c>
-      <c r="C12" t="s">
-        <v>81</v>
-      </c>
       <c r="D12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1619,19 +1619,19 @@
         <v>50</v>
       </c>
       <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
         <v>82</v>
       </c>
-      <c r="C13" t="s">
-        <v>83</v>
-      </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished emulation feasibility part
</commit_message>
<xml_diff>
--- a/tables/helper_tables.xlsx
+++ b/tables/helper_tables.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janickweberpals/Documents/Projects/encore-process-paper/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E176BD46-8E3E-4C4B-99EB-8B2198800D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72D5B82-485B-6C49-B914-49866975AF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ctgov_criteria_defintions" sheetId="1" r:id="rId1"/>
     <sheet name="rct_selection" sheetId="2" r:id="rId2"/>
+    <sheet name="databases" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="115">
   <si>
     <t>Criteria</t>
   </si>
@@ -339,6 +340,40 @@
   </si>
   <si>
     <t>Metastatic squamous/non-squamous</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>COTA</t>
+  </si>
+  <si>
+    <t>ConcertAI</t>
+  </si>
+  <si>
+    <t>Flatiron health</t>
+  </si>
+  <si>
+    <t>Ontada</t>
+  </si>
+  <si>
+    <t>Patient identification period</t>
+  </si>
+  <si>
+    <t>Follow-up through</t>
+  </si>
+  <si>
+    <t>January 1, 2011 - April 30, 2024</t>
+  </si>
+  <si>
+    <t>April 30, 2024</t>
+  </si>
+  <si>
+    <t>US Oncology Network iKnowMed™(iKM)
+electronic health record (EHR) system, an integrated web-based database and oncology-specific EHR system that captures outpatient practice
+encounter histories from network community oncology practices affiliated with
+over 1,000 physicians in more than 25 practices across 400 sites of care in 19
+states</t>
   </si>
 </sst>
 </file>
@@ -822,7 +857,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -831,6 +866,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1360,7 +1405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6A9B8D-1FAF-D141-AC37-A562D99120E8}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1637,4 +1682,97 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0803B4C0-E798-1D4C-A3E2-DEC3AF4949CE}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="221" zoomScaleNormal="221" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
additions on runner up clinical trial candidates for emulation
</commit_message>
<xml_diff>
--- a/tables/helper_tables.xlsx
+++ b/tables/helper_tables.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janickweberpals/Documents/Projects/encore-process-paper/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBAE143-22A8-034A-8FCD-13095990B7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A55F59-4951-0048-A47B-BE289312DCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="26540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ctgov_criteria_defintions" sheetId="1" r:id="rId1"/>
-    <sheet name="rct_selection" sheetId="2" r:id="rId2"/>
-    <sheet name="databases" sheetId="3" r:id="rId3"/>
+    <sheet name="runner_ups" sheetId="4" r:id="rId2"/>
+    <sheet name="rct_selection" sheetId="2" r:id="rId3"/>
+    <sheet name="databases" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="161">
   <si>
     <t>Criteria</t>
   </si>
@@ -375,12 +376,150 @@
 over 1,000 physicians in more than 25 practices across 400 sites of care in 19
 states</t>
   </si>
+  <si>
+    <t>NCT02220894</t>
+  </si>
+  <si>
+    <t>KEYNOTE-042</t>
+  </si>
+  <si>
+    <t>NCT02125461</t>
+  </si>
+  <si>
+    <t>PACIFIC</t>
+  </si>
+  <si>
+    <t>NCT02578680</t>
+  </si>
+  <si>
+    <t>KEYNOTE-189</t>
+  </si>
+  <si>
+    <t>NCT02775435</t>
+  </si>
+  <si>
+    <t>KEYNOTE-407</t>
+  </si>
+  <si>
+    <t>MONALEESA-2</t>
+  </si>
+  <si>
+    <t>CLEOPATRA</t>
+  </si>
+  <si>
+    <t>MONARCH-3</t>
+  </si>
+  <si>
+    <t>NALA</t>
+  </si>
+  <si>
+    <t>Locally advanced/metastatic non-small-cell lung cancer (NSCLC) without EGFR/ALK alterations and with programmed death ligand-1 (PD-L1) tumor proportion score (TPS) ≥ 1%</t>
+  </si>
+  <si>
+    <t>Stage III non-small-cell lung cancer and no disease progression after concurrent chemoradiotherapy.</t>
+  </si>
+  <si>
+    <t>durvalumab versus placebo</t>
+  </si>
+  <si>
+    <t>Unresectable, stage III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metastatic nonsquamous non-small-cell lung cancer without EGFR/ALK alterations </t>
+  </si>
+  <si>
+    <t>NCT01958021</t>
+  </si>
+  <si>
+    <t>Metastatic squamous non–small-cell lung cancer (NSCLC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pembrolizumab or placebo plus carboplatin and paclitaxel/nab-paclitaxel </t>
+  </si>
+  <si>
+    <t>pemetrexed plus platinum with or without pembrolizumab</t>
+  </si>
+  <si>
+    <t>pembrolizumab monotherapy to standard platinum-based chemotherapy</t>
+  </si>
+  <si>
+    <t>Postmenopausal HR-positive/HER2-negative advanced or metastatic breast cancer</t>
+  </si>
+  <si>
+    <t>ribociclib plus letrozole versus placebo plus letrozole</t>
+  </si>
+  <si>
+    <t>Postmenopausal HR-positive/HER2-negative locoregionally recurrent or metastatic breast cancer</t>
+  </si>
+  <si>
+    <t>NCT02246621</t>
+  </si>
+  <si>
+    <t>abemaciclib plus nonsteroidal aromatase inhibitor (NSAI; anastrozole or letrozole) versus placebo plus NSAI (anastrozole or letrozole)</t>
+  </si>
+  <si>
+    <t>neratinib plus capecitabine versus lapatinib plus capecitabine</t>
+  </si>
+  <si>
+    <t>HER2-positive (HER2+) metastatic breast cancer</t>
+  </si>
+  <si>
+    <t>3L+</t>
+  </si>
+  <si>
+    <t>NCT01808573</t>
+  </si>
+  <si>
+    <t>NCT00567190</t>
+  </si>
+  <si>
+    <t>pertuzumab plus trastuzumab and docetaxel versus placebo plus trastuzumab and docetaxel</t>
+  </si>
+  <si>
+    <t>1L (one prior hormonal treatment for metastatic breast cancer was allowed)</t>
+  </si>
+  <si>
+    <t>NCT01607957</t>
+  </si>
+  <si>
+    <t>Refractory metastatic colorectal cancer</t>
+  </si>
+  <si>
+    <t>RECOURSE</t>
+  </si>
+  <si>
+    <t>trifluridine/tipiracil plus best supportive care versus placebo plus best supportive care</t>
+  </si>
+  <si>
+    <t>GRIFFIN</t>
+  </si>
+  <si>
+    <t>NCT02874742</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transplant-eligible, newly diagnosed multiple myeloma </t>
+  </si>
+  <si>
+    <t>daratumumab, lenalidomide, bortezomib, and dexamethasone (induction, consolidation) followed by daratumumab plus lenalidomide (maintenance) versus lenalidomide, bortezomib, and dexamethasone (induction, consolidation) followed by lenalidomide (maintenance)</t>
+  </si>
+  <si>
+    <t>NCT02076009</t>
+  </si>
+  <si>
+    <t>POLLUX</t>
+  </si>
+  <si>
+    <t>daratumumab plus lenalidomide and dexamethasone versus lenalidomide plus dexamethasone</t>
+  </si>
+  <si>
+    <t>Relapsed/refractory multiple myeloma</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -515,6 +654,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -813,7 +960,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -856,8 +1003,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -876,8 +1024,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -911,6 +1071,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1233,7 +1394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1402,12 +1563,285 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B7B560-98D0-F74F-886E-42E449BB416A}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="179" zoomScaleNormal="179" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5" style="10" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.1640625" style="10" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="136" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display=" NCT01958021" xr:uid="{07981B6E-3A1D-D64D-A8B1-466F993EA216}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{720E312A-AF4C-EC4C-8423-5DF21FFF76AC}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{46E43196-9119-9C4F-9CB8-9FDF09B67989}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{9EEDE2D6-31EE-F041-8B60-60BCA1CD7ADF}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{CA0B80B4-F60C-0A4C-B32E-2597949D7BE2}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{66D865F8-7DA5-A04D-99F5-97AF9593EDA9}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{BDDB669D-8E97-AC4D-88E9-30A72F5B7210}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{2C010ED7-39AC-B44F-9A3C-4FC8B8C5AEDE}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{0AF5BA8C-BBF0-EE47-8810-B3029E8BCAE4}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{BC60402E-F322-234C-BCD8-9690841C0E0C}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{C1F38E0A-55FF-E241-9266-17EE5452BD21}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6A9B8D-1FAF-D141-AC37-A562D99120E8}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1684,7 +2118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0803B4C0-E798-1D4C-A3E2-DEC3AF4949CE}">
   <dimension ref="A1:F7"/>
   <sheetViews>

</xml_diff>